<commit_message>
Rotate each terminal to try to find a slightly better connection
</commit_message>
<xml_diff>
--- a/src/PumpjackPipeOptimizer/Comparison.xlsx
+++ b/src/PumpjackPipeOptimizer/Comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joelv\Desktop\PumpjackPipeOptimizer\src\PumpjackPipeOptimizer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z\GitHub\joelverhagen\FactorioTools\src\PumpjackPipeOptimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79FED07-1CDF-4377-8535-11B03F073AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8785628F-D891-4208-9F0E-29AE294F40FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-210" windowWidth="29040" windowHeight="15720" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>FBE</t>
   </si>
@@ -100,6 +100,30 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>a8f549899c571087d9aec80fe95576e3f725c978</t>
+  </si>
+  <si>
+    <t>Shorter trunks</t>
+  </si>
+  <si>
+    <t>Prefer close to neighbor centroid</t>
+  </si>
+  <si>
+    <t>b840958b77288d75161e9e8ba958e8d3c4072c36</t>
+  </si>
+  <si>
+    <t>a146f34768acb02954a0a3bc4f3ad76126a94ec0</t>
+  </si>
+  <si>
+    <t>Don't let trunks overlap</t>
+  </si>
+  <si>
+    <t>Prefer paths that snap to pumpjack sides</t>
+  </si>
+  <si>
+    <t>0007e275b2bca5858cc5209e196e5b66ba35be6f</t>
+  </si>
 </sst>
 </file>
 
@@ -151,29 +175,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -504,24 +516,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EBF3A-B501-4205-AA83-0ECFC9C1E5B1}">
-  <dimension ref="A1:L61"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.86328125" customWidth="1"/>
+    <col min="9" max="9" width="8.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -551,10 +563,22 @@
       <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -584,13 +608,25 @@
       <c r="K2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>0</v>
       </c>
-      <c r="B3" s="6">
-        <f>MIN(C3:K3)</f>
+      <c r="B3">
+        <f>MIN(C3:O3)</f>
         <v>16</v>
       </c>
       <c r="C3">
@@ -621,16 +657,28 @@
         <v>16</v>
       </c>
       <c r="L3">
-        <f>K3-B3</f>
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
+      <c r="O3">
+        <v>16</v>
+      </c>
+      <c r="P3">
+        <f>N3-B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="6">
-        <f>MIN(C4:K4)</f>
+      <c r="B4">
+        <f t="shared" ref="B4:B60" si="0">MIN(C4:O4)</f>
         <v>121</v>
       </c>
       <c r="C4">
@@ -661,16 +709,28 @@
         <v>121</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L60" si="0">K4-B4</f>
+        <v>125</v>
+      </c>
+      <c r="M4">
+        <v>121</v>
+      </c>
+      <c r="N4">
+        <v>121</v>
+      </c>
+      <c r="O4">
+        <v>121</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P60" si="1">N4-B4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="6">
-        <f>MIN(C5:K5)</f>
+      <c r="B5">
+        <f t="shared" si="0"/>
         <v>99</v>
       </c>
       <c r="C5">
@@ -701,17 +761,29 @@
         <v>99</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="M5">
+        <v>109</v>
+      </c>
+      <c r="N5">
+        <v>109</v>
+      </c>
+      <c r="O5">
+        <v>111</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="6">
-        <f>MIN(C6:K6)</f>
-        <v>80</v>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>90</v>
@@ -741,17 +813,29 @@
         <v>83</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="M6">
+        <v>78</v>
+      </c>
+      <c r="N6">
+        <v>78</v>
+      </c>
+      <c r="O6">
+        <v>78</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="6">
-        <f>MIN(C7:K7)</f>
-        <v>84</v>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>83</v>
       </c>
       <c r="C7">
         <v>84</v>
@@ -781,16 +865,28 @@
         <v>88</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="M7">
+        <v>83</v>
+      </c>
+      <c r="N7">
+        <v>83</v>
+      </c>
+      <c r="O7">
+        <v>83</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="6">
-        <f>MIN(C8:K8)</f>
+      <c r="B8">
+        <f t="shared" si="0"/>
         <v>77</v>
       </c>
       <c r="C8">
@@ -821,16 +917,28 @@
         <v>82</v>
       </c>
       <c r="L8">
-        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="M8">
+        <v>82</v>
+      </c>
+      <c r="N8">
+        <v>82</v>
+      </c>
+      <c r="O8">
+        <v>82</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="6">
-        <f>MIN(C9:K9)</f>
+      <c r="B9">
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="C9">
@@ -861,17 +969,29 @@
         <v>97</v>
       </c>
       <c r="L9">
-        <f t="shared" si="0"/>
+        <v>97</v>
+      </c>
+      <c r="M9">
+        <v>97</v>
+      </c>
+      <c r="N9">
+        <v>97</v>
+      </c>
+      <c r="O9">
+        <v>97</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
-        <f>MIN(C10:K10)</f>
-        <v>67</v>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>82</v>
@@ -901,17 +1021,29 @@
         <v>73</v>
       </c>
       <c r="L10">
-        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="M10">
+        <v>71</v>
+      </c>
+      <c r="N10">
+        <v>71</v>
+      </c>
+      <c r="O10">
+        <v>71</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="6">
-        <f>MIN(C11:K11)</f>
-        <v>89</v>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>88</v>
       </c>
       <c r="C11">
         <v>95</v>
@@ -941,16 +1073,28 @@
         <v>89</v>
       </c>
       <c r="L11">
-        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+      <c r="M11">
+        <v>88</v>
+      </c>
+      <c r="N11">
+        <v>88</v>
+      </c>
+      <c r="O11">
+        <v>88</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>9</v>
       </c>
-      <c r="B12" s="6">
-        <f>MIN(C12:K12)</f>
+      <c r="B12">
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="C12">
@@ -981,16 +1125,28 @@
         <v>117</v>
       </c>
       <c r="L12">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="M12">
+        <v>107</v>
+      </c>
+      <c r="N12">
+        <v>103</v>
+      </c>
+      <c r="O12">
+        <v>103</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
-        <f>MIN(C13:K13)</f>
+      <c r="B13">
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="C13">
@@ -1021,16 +1177,28 @@
         <v>108</v>
       </c>
       <c r="L13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="M13">
+        <v>109</v>
+      </c>
+      <c r="N13">
+        <v>109</v>
+      </c>
+      <c r="O13">
+        <v>109</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
-        <f>MIN(C14:K14)</f>
+      <c r="B14">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C14">
@@ -1061,16 +1229,28 @@
         <v>54</v>
       </c>
       <c r="L14">
-        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="M14">
+        <v>54</v>
+      </c>
+      <c r="N14">
+        <v>54</v>
+      </c>
+      <c r="O14">
+        <v>54</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>12</v>
       </c>
-      <c r="B15" s="6">
-        <f>MIN(C15:K15)</f>
+      <c r="B15">
+        <f t="shared" si="0"/>
         <v>76</v>
       </c>
       <c r="C15">
@@ -1101,16 +1281,28 @@
         <v>76</v>
       </c>
       <c r="L15">
-        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="M15">
+        <v>76</v>
+      </c>
+      <c r="N15">
+        <v>76</v>
+      </c>
+      <c r="O15">
+        <v>76</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>13</v>
       </c>
-      <c r="B16" s="6">
-        <f>MIN(C16:K16)</f>
+      <c r="B16">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="C16">
@@ -1141,16 +1333,28 @@
         <v>93</v>
       </c>
       <c r="L16">
-        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="M16">
+        <v>93</v>
+      </c>
+      <c r="N16">
+        <v>93</v>
+      </c>
+      <c r="O16">
+        <v>93</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>14</v>
       </c>
-      <c r="B17" s="6">
-        <f>MIN(C17:K17)</f>
+      <c r="B17">
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="C17">
@@ -1181,16 +1385,28 @@
         <v>76</v>
       </c>
       <c r="L17">
-        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="M17">
+        <v>76</v>
+      </c>
+      <c r="N17">
+        <v>76</v>
+      </c>
+      <c r="O17">
+        <v>75</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>15</v>
       </c>
-      <c r="B18" s="6">
-        <f>MIN(C18:K18)</f>
+      <c r="B18">
+        <f t="shared" si="0"/>
         <v>80</v>
       </c>
       <c r="C18">
@@ -1221,16 +1437,28 @@
         <v>80</v>
       </c>
       <c r="L18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="M18">
+        <v>84</v>
+      </c>
+      <c r="N18">
+        <v>84</v>
+      </c>
+      <c r="O18">
+        <v>84</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>16</v>
       </c>
-      <c r="B19" s="6">
-        <f>MIN(C19:K19)</f>
+      <c r="B19">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="C19">
@@ -1261,16 +1489,28 @@
         <v>32</v>
       </c>
       <c r="L19">
-        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M19">
+        <v>32</v>
+      </c>
+      <c r="N19">
+        <v>32</v>
+      </c>
+      <c r="O19">
+        <v>32</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>17</v>
       </c>
-      <c r="B20" s="6">
-        <f>MIN(C20:K20)</f>
+      <c r="B20">
+        <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="C20">
@@ -1301,16 +1541,28 @@
         <v>37</v>
       </c>
       <c r="L20">
-        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="M20">
+        <v>37</v>
+      </c>
+      <c r="N20">
+        <v>37</v>
+      </c>
+      <c r="O20">
+        <v>37</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>18</v>
       </c>
-      <c r="B21" s="6">
-        <f>MIN(C21:K21)</f>
+      <c r="B21">
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="C21">
@@ -1341,16 +1593,28 @@
         <v>32</v>
       </c>
       <c r="L21">
-        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="M21">
+        <v>32</v>
+      </c>
+      <c r="N21">
+        <v>32</v>
+      </c>
+      <c r="O21">
+        <v>32</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>19</v>
       </c>
-      <c r="B22" s="6">
-        <f>MIN(C22:K22)</f>
+      <c r="B22">
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C22">
@@ -1381,16 +1645,28 @@
         <v>49</v>
       </c>
       <c r="L22">
-        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="M22">
+        <v>49</v>
+      </c>
+      <c r="N22">
+        <v>49</v>
+      </c>
+      <c r="O22">
+        <v>49</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>20</v>
       </c>
-      <c r="B23" s="6">
-        <f>MIN(C23:K23)</f>
+      <c r="B23">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C23">
@@ -1421,16 +1697,28 @@
         <v>14</v>
       </c>
       <c r="L23">
-        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="M23">
+        <v>14</v>
+      </c>
+      <c r="N23">
+        <v>14</v>
+      </c>
+      <c r="O23">
+        <v>14</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>21</v>
       </c>
-      <c r="B24" s="6">
-        <f>MIN(C24:K24)</f>
+      <c r="B24">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C24">
@@ -1461,16 +1749,28 @@
         <v>58</v>
       </c>
       <c r="L24">
-        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="M24">
+        <v>58</v>
+      </c>
+      <c r="N24">
+        <v>58</v>
+      </c>
+      <c r="O24">
+        <v>57</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>22</v>
       </c>
-      <c r="B25" s="6">
-        <f>MIN(C25:K25)</f>
+      <c r="B25">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
       <c r="C25">
@@ -1501,16 +1801,28 @@
         <v>67</v>
       </c>
       <c r="L25">
-        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="M25">
+        <v>67</v>
+      </c>
+      <c r="N25">
+        <v>67</v>
+      </c>
+      <c r="O25">
+        <v>67</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>23</v>
       </c>
-      <c r="B26" s="6">
-        <f>MIN(C26:K26)</f>
+      <c r="B26">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C26">
@@ -1541,16 +1853,28 @@
         <v>29</v>
       </c>
       <c r="L26">
-        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="M26">
+        <v>29</v>
+      </c>
+      <c r="N26">
+        <v>29</v>
+      </c>
+      <c r="O26">
+        <v>29</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>24</v>
       </c>
-      <c r="B27" s="6">
-        <f>MIN(C27:K27)</f>
+      <c r="B27">
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C27">
@@ -1581,17 +1905,29 @@
         <v>29</v>
       </c>
       <c r="L27">
-        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="M27">
+        <v>29</v>
+      </c>
+      <c r="N27">
+        <v>29</v>
+      </c>
+      <c r="O27">
+        <v>29</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>25</v>
       </c>
-      <c r="B28" s="6">
-        <f>MIN(C28:K28)</f>
-        <v>69</v>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>66</v>
       </c>
       <c r="C28">
         <v>70</v>
@@ -1621,16 +1957,28 @@
         <v>77</v>
       </c>
       <c r="L28">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="M28">
+        <v>66</v>
+      </c>
+      <c r="N28">
+        <v>66</v>
+      </c>
+      <c r="O28">
+        <v>66</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>26</v>
       </c>
-      <c r="B29" s="6">
-        <f>MIN(C29:K29)</f>
+      <c r="B29">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="C29">
@@ -1661,16 +2009,28 @@
         <v>51</v>
       </c>
       <c r="L29">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="M29">
+        <v>47</v>
+      </c>
+      <c r="N29">
+        <v>47</v>
+      </c>
+      <c r="O29">
+        <v>47</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>27</v>
       </c>
-      <c r="B30" s="6">
-        <f>MIN(C30:K30)</f>
+      <c r="B30">
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="C30">
@@ -1701,16 +2061,28 @@
         <v>45</v>
       </c>
       <c r="L30">
-        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="M30">
+        <v>45</v>
+      </c>
+      <c r="N30">
+        <v>45</v>
+      </c>
+      <c r="O30">
+        <v>45</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>28</v>
       </c>
-      <c r="B31" s="6">
-        <f>MIN(C31:K31)</f>
+      <c r="B31">
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="C31">
@@ -1741,16 +2113,28 @@
         <v>87</v>
       </c>
       <c r="L31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="M31">
+        <v>88</v>
+      </c>
+      <c r="N31">
+        <v>88</v>
+      </c>
+      <c r="O31">
+        <v>87</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>29</v>
       </c>
-      <c r="B32" s="6">
-        <f>MIN(C32:K32)</f>
+      <c r="B32">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C32">
@@ -1781,16 +2165,28 @@
         <v>58</v>
       </c>
       <c r="L32">
-        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="M32">
+        <v>58</v>
+      </c>
+      <c r="N32">
+        <v>58</v>
+      </c>
+      <c r="O32">
+        <v>58</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>30</v>
       </c>
-      <c r="B33" s="6">
-        <f>MIN(C33:K33)</f>
+      <c r="B33">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
       <c r="C33">
@@ -1821,16 +2217,28 @@
         <v>75</v>
       </c>
       <c r="L33">
-        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="M33">
+        <v>75</v>
+      </c>
+      <c r="N33">
+        <v>75</v>
+      </c>
+      <c r="O33">
+        <v>75</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>31</v>
       </c>
-      <c r="B34" s="6">
-        <f>MIN(C34:K34)</f>
+      <c r="B34">
+        <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C34">
@@ -1861,17 +2269,29 @@
         <v>62</v>
       </c>
       <c r="L34">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="M34">
+        <v>59</v>
+      </c>
+      <c r="N34">
+        <v>59</v>
+      </c>
+      <c r="O34">
+        <v>59</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>32</v>
       </c>
-      <c r="B35" s="6">
-        <f>MIN(C35:K35)</f>
-        <v>45</v>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="C35">
         <v>46</v>
@@ -1901,16 +2321,28 @@
         <v>51</v>
       </c>
       <c r="L35">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="M35">
+        <v>44</v>
+      </c>
+      <c r="N35">
+        <v>44</v>
+      </c>
+      <c r="O35">
+        <v>44</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>33</v>
       </c>
-      <c r="B36" s="6">
-        <f>MIN(C36:K36)</f>
+      <c r="B36">
+        <f t="shared" si="0"/>
         <v>130</v>
       </c>
       <c r="C36">
@@ -1941,16 +2373,28 @@
         <v>136</v>
       </c>
       <c r="L36">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="M36">
+        <v>131</v>
+      </c>
+      <c r="N36">
+        <v>131</v>
+      </c>
+      <c r="O36">
+        <v>130</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>34</v>
       </c>
-      <c r="B37" s="6">
-        <f>MIN(C37:K37)</f>
+      <c r="B37">
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
       <c r="C37">
@@ -1981,16 +2425,28 @@
         <v>154</v>
       </c>
       <c r="L37">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="M37">
+        <v>146</v>
+      </c>
+      <c r="N37">
+        <v>146</v>
+      </c>
+      <c r="O37">
+        <v>146</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>35</v>
       </c>
-      <c r="B38" s="6">
-        <f>MIN(C38:K38)</f>
+      <c r="B38">
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
       <c r="C38">
@@ -2021,16 +2477,28 @@
         <v>83</v>
       </c>
       <c r="L38">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="M38">
+        <v>81</v>
+      </c>
+      <c r="N38">
+        <v>81</v>
+      </c>
+      <c r="O38">
+        <v>81</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>36</v>
       </c>
-      <c r="B39" s="6">
-        <f>MIN(C39:K39)</f>
+      <c r="B39">
+        <f t="shared" si="0"/>
         <v>93</v>
       </c>
       <c r="C39">
@@ -2061,17 +2529,29 @@
         <v>98</v>
       </c>
       <c r="L39">
-        <f t="shared" si="0"/>
+        <v>98</v>
+      </c>
+      <c r="M39">
+        <v>98</v>
+      </c>
+      <c r="N39">
+        <v>98</v>
+      </c>
+      <c r="O39">
+        <v>96</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>37</v>
       </c>
-      <c r="B40" s="6">
-        <f>MIN(C40:K40)</f>
-        <v>90</v>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>88</v>
       </c>
       <c r="C40">
         <v>99</v>
@@ -2101,17 +2581,29 @@
         <v>91</v>
       </c>
       <c r="L40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="M40">
+        <v>88</v>
+      </c>
+      <c r="N40">
+        <v>88</v>
+      </c>
+      <c r="O40">
+        <v>90</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>38</v>
       </c>
-      <c r="B41" s="6">
-        <f>MIN(C41:K41)</f>
-        <v>82</v>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>81</v>
       </c>
       <c r="C41">
         <v>91</v>
@@ -2141,16 +2633,28 @@
         <v>82</v>
       </c>
       <c r="L41">
-        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="M41">
+        <v>81</v>
+      </c>
+      <c r="N41">
+        <v>81</v>
+      </c>
+      <c r="O41">
+        <v>84</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>39</v>
       </c>
-      <c r="B42" s="6">
-        <f>MIN(C42:K42)</f>
+      <c r="B42">
+        <f t="shared" si="0"/>
         <v>91</v>
       </c>
       <c r="C42">
@@ -2181,16 +2685,28 @@
         <v>95</v>
       </c>
       <c r="L42">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="M42">
+        <v>92</v>
+      </c>
+      <c r="N42">
+        <v>92</v>
+      </c>
+      <c r="O42">
+        <v>92</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>40</v>
       </c>
-      <c r="B43" s="6">
-        <f>MIN(C43:K43)</f>
+      <c r="B43">
+        <f t="shared" si="0"/>
         <v>116</v>
       </c>
       <c r="C43">
@@ -2221,16 +2737,28 @@
         <v>125</v>
       </c>
       <c r="L43">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="M43">
+        <v>134</v>
+      </c>
+      <c r="N43">
+        <v>134</v>
+      </c>
+      <c r="O43">
+        <v>124</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>41</v>
       </c>
-      <c r="B44" s="6">
-        <f>MIN(C44:K44)</f>
+      <c r="B44">
+        <f t="shared" si="0"/>
         <v>103</v>
       </c>
       <c r="C44">
@@ -2261,17 +2789,29 @@
         <v>113</v>
       </c>
       <c r="L44">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="M44">
+        <v>108</v>
+      </c>
+      <c r="N44">
+        <v>108</v>
+      </c>
+      <c r="O44">
+        <v>107</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>42</v>
       </c>
-      <c r="B45" s="6">
-        <f>MIN(C45:K45)</f>
-        <v>123</v>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>122</v>
       </c>
       <c r="C45">
         <v>133</v>
@@ -2301,16 +2841,28 @@
         <v>123</v>
       </c>
       <c r="L45">
-        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="M45">
+        <v>122</v>
+      </c>
+      <c r="N45">
+        <v>122</v>
+      </c>
+      <c r="O45">
+        <v>122</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>43</v>
       </c>
-      <c r="B46" s="6">
-        <f>MIN(C46:K46)</f>
+      <c r="B46">
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="C46">
@@ -2341,16 +2893,28 @@
         <v>128</v>
       </c>
       <c r="L46">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="M46">
+        <v>125</v>
+      </c>
+      <c r="N46">
+        <v>125</v>
+      </c>
+      <c r="O46">
+        <v>125</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>44</v>
       </c>
-      <c r="B47" s="6">
-        <f>MIN(C47:K47)</f>
+      <c r="B47">
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="C47">
@@ -2381,16 +2945,28 @@
         <v>105</v>
       </c>
       <c r="L47">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="M47">
+        <v>98</v>
+      </c>
+      <c r="N47">
+        <v>98</v>
+      </c>
+      <c r="O47">
+        <v>98</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>45</v>
       </c>
-      <c r="B48" s="6">
-        <f>MIN(C48:K48)</f>
+      <c r="B48">
+        <f t="shared" si="0"/>
         <v>111</v>
       </c>
       <c r="C48">
@@ -2421,16 +2997,28 @@
         <v>121</v>
       </c>
       <c r="L48">
-        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="M48">
+        <v>121</v>
+      </c>
+      <c r="N48">
+        <v>121</v>
+      </c>
+      <c r="O48">
+        <v>121</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>46</v>
       </c>
-      <c r="B49" s="6">
-        <f>MIN(C49:K49)</f>
+      <c r="B49">
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="C49">
@@ -2461,16 +3049,28 @@
         <v>115</v>
       </c>
       <c r="L49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="M49">
+        <v>120</v>
+      </c>
+      <c r="N49">
+        <v>120</v>
+      </c>
+      <c r="O49">
+        <v>120</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>47</v>
       </c>
-      <c r="B50" s="6">
-        <f>MIN(C50:K50)</f>
+      <c r="B50">
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="C50">
@@ -2501,16 +3101,28 @@
         <v>132</v>
       </c>
       <c r="L50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="M50">
+        <v>140</v>
+      </c>
+      <c r="N50">
+        <v>140</v>
+      </c>
+      <c r="O50">
+        <v>135</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>48</v>
       </c>
-      <c r="B51" s="6">
-        <f>MIN(C51:K51)</f>
+      <c r="B51">
+        <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="C51">
@@ -2541,17 +3153,29 @@
         <v>94</v>
       </c>
       <c r="L51">
-        <f t="shared" si="0"/>
+        <v>94</v>
+      </c>
+      <c r="M51">
+        <v>94</v>
+      </c>
+      <c r="N51">
+        <v>94</v>
+      </c>
+      <c r="O51">
+        <v>94</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>49</v>
       </c>
-      <c r="B52" s="6">
-        <f>MIN(C52:K52)</f>
-        <v>124</v>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>122</v>
       </c>
       <c r="C52">
         <v>138</v>
@@ -2581,16 +3205,28 @@
         <v>125</v>
       </c>
       <c r="L52">
-        <f t="shared" si="0"/>
+        <v>123</v>
+      </c>
+      <c r="M52">
+        <v>123</v>
+      </c>
+      <c r="N52">
+        <v>123</v>
+      </c>
+      <c r="O52">
+        <v>122</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>50</v>
       </c>
-      <c r="B53" s="6">
-        <f>MIN(C53:K53)</f>
+      <c r="B53">
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="C53">
@@ -2621,17 +3257,29 @@
         <v>118</v>
       </c>
       <c r="L53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="M53">
+        <v>119</v>
+      </c>
+      <c r="N53">
+        <v>119</v>
+      </c>
+      <c r="O53">
+        <v>119</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>51</v>
       </c>
-      <c r="B54" s="6">
-        <f>MIN(C54:K54)</f>
-        <v>175</v>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>171</v>
       </c>
       <c r="C54">
         <v>195</v>
@@ -2661,16 +3309,28 @@
         <v>178</v>
       </c>
       <c r="L54">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="M54">
+        <v>172</v>
+      </c>
+      <c r="N54">
+        <v>172</v>
+      </c>
+      <c r="O54">
+        <v>171</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>52</v>
       </c>
-      <c r="B55" s="6">
-        <f>MIN(C55:K55)</f>
+      <c r="B55">
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
       <c r="C55">
@@ -2701,16 +3361,28 @@
         <v>150</v>
       </c>
       <c r="L55">
-        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="M55">
+        <v>150</v>
+      </c>
+      <c r="N55">
+        <v>150</v>
+      </c>
+      <c r="O55">
+        <v>150</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>53</v>
       </c>
-      <c r="B56" s="6">
-        <f>MIN(C56:K56)</f>
+      <c r="B56">
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="C56">
@@ -2741,17 +3413,29 @@
         <v>104</v>
       </c>
       <c r="L56">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="M56">
+        <v>103</v>
+      </c>
+      <c r="N56">
+        <v>103</v>
+      </c>
+      <c r="O56">
+        <v>102</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>54</v>
       </c>
-      <c r="B57" s="6">
-        <f>MIN(C57:K57)</f>
-        <v>114</v>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>113</v>
       </c>
       <c r="C57">
         <v>121</v>
@@ -2781,16 +3465,28 @@
         <v>114</v>
       </c>
       <c r="L57">
-        <f t="shared" si="0"/>
+        <v>116</v>
+      </c>
+      <c r="M57">
+        <v>113</v>
+      </c>
+      <c r="N57">
+        <v>113</v>
+      </c>
+      <c r="O57">
+        <v>113</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>55</v>
       </c>
-      <c r="B58" s="6">
-        <f>MIN(C58:K58)</f>
+      <c r="B58">
+        <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="C58">
@@ -2821,16 +3517,28 @@
         <v>108</v>
       </c>
       <c r="L58">
-        <f t="shared" si="0"/>
+        <v>108</v>
+      </c>
+      <c r="M58">
+        <v>108</v>
+      </c>
+      <c r="N58">
+        <v>108</v>
+      </c>
+      <c r="O58">
+        <v>111</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>56</v>
       </c>
-      <c r="B59" s="6">
-        <f>MIN(C59:K59)</f>
+      <c r="B59">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="C59">
@@ -2861,16 +3569,28 @@
         <v>121</v>
       </c>
       <c r="L59">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="M59">
+        <v>122</v>
+      </c>
+      <c r="N59">
+        <v>122</v>
+      </c>
+      <c r="O59">
+        <v>121</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>57</v>
       </c>
-      <c r="B60" s="6">
-        <f>MIN(C60:K60)</f>
+      <c r="B60">
+        <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="C60">
@@ -2901,11 +3621,23 @@
         <v>131</v>
       </c>
       <c r="L60">
-        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="M60">
+        <v>131</v>
+      </c>
+      <c r="N60">
+        <v>131</v>
+      </c>
+      <c r="O60">
+        <v>131</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
       <c r="C61">
         <v>93.396551724137893</v>
       </c>
@@ -2914,40 +3646,58 @@
         <v>92.068965517241381</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:J61" si="1">AVERAGE(E3:E60)</f>
+        <f t="shared" ref="E61:P61" si="2">AVERAGE(E3:E60)</f>
         <v>92.793103448275858</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.827586206896555</v>
       </c>
       <c r="G61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.965517241379317</v>
       </c>
       <c r="H61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90.120689655172413</v>
       </c>
       <c r="I61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>89.965517241379317</v>
       </c>
       <c r="J61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90.224137931034477</v>
       </c>
       <c r="K61">
-        <v>88.775862068965495</v>
+        <f t="shared" si="2"/>
+        <v>88.775862068965523</v>
+      </c>
+      <c r="L61">
+        <f t="shared" si="2"/>
+        <v>88.568965517241381</v>
+      </c>
+      <c r="M61">
+        <v>87.810344827586206</v>
+      </c>
+      <c r="N61">
+        <v>87.741379310344797</v>
+      </c>
+      <c r="O61">
+        <v>87.465517241379303</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="2"/>
+        <v>2.2413793103448274</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:K1048576">
+  <conditionalFormatting sqref="C1:O60 C62:O1048576 C61:P61">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), 2)) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:K4">
+  <conditionalFormatting sqref="C4:O4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$B$3</formula>
     </cfRule>
@@ -2955,4 +3705,10 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f42aa342-8706-4288-bd11-ebb85995028c}" enabled="1" method="Standard" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Add latest comparison data
</commit_message>
<xml_diff>
--- a/src/PumpjackPipeOptimizer/Comparison.xlsx
+++ b/src/PumpjackPipeOptimizer/Comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\z\GitHub\joelverhagen\FactorioTools\src\PumpjackPipeOptimizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8785628F-D891-4208-9F0E-29AE294F40FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE764A9-1E30-4127-B4E1-16DC64938485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{F3EEF332-D963-44B3-89AD-4C5E1973BCE9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>FBE</t>
   </si>
@@ -123,6 +123,15 @@
   </si>
   <si>
     <t>0007e275b2bca5858cc5209e196e5b66ba35be6f</t>
+  </si>
+  <si>
+    <t>6895266baf0a232e390f5673bf0036f9ea6ccdf7</t>
+  </si>
+  <si>
+    <t>Rotate each terminal to try to find a slightly better connection</t>
+  </si>
+  <si>
+    <t>9d8a0295d946bdc2c57a606ba1376d2a8734b586</t>
   </si>
 </sst>
 </file>
@@ -516,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0EBF3A-B501-4205-AA83-0ECFC9C1E5B1}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="R38" sqref="R38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -529,7 +538,7 @@
     <col min="9" max="9" width="8.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -575,8 +584,11 @@
       <c r="O1" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="P1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>20</v>
@@ -620,13 +632,19 @@
       <c r="O2" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3">
-        <f>MIN(C3:O3)</f>
+        <f>MIN(C3:Q3)</f>
         <v>16</v>
       </c>
       <c r="C3">
@@ -669,16 +687,22 @@
         <v>16</v>
       </c>
       <c r="P3">
-        <f>N3-B3</f>
+        <v>16</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <f>Q3-B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B60" si="0">MIN(C4:O4)</f>
+        <f t="shared" ref="B4:B60" si="0">MIN(C4:Q4)</f>
         <v>121</v>
       </c>
       <c r="C4">
@@ -721,17 +745,23 @@
         <v>121</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P60" si="1">N4-B4</f>
+        <v>121</v>
+      </c>
+      <c r="Q4">
+        <v>121</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ref="R4:R60" si="1">Q4-B4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5">
         <v>113</v>
@@ -773,11 +803,17 @@
         <v>111</v>
       </c>
       <c r="P5">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+        <v>110</v>
+      </c>
+      <c r="Q5">
+        <v>95</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -825,11 +861,17 @@
         <v>78</v>
       </c>
       <c r="P6">
+        <v>78</v>
+      </c>
+      <c r="Q6">
+        <v>78</v>
+      </c>
+      <c r="R6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -877,17 +919,23 @@
         <v>83</v>
       </c>
       <c r="P7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+      <c r="Q7">
+        <v>84</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C8">
         <v>80</v>
@@ -929,17 +977,23 @@
         <v>82</v>
       </c>
       <c r="P8">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+      <c r="Q8">
+        <v>73</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <v>96</v>
@@ -981,11 +1035,17 @@
         <v>97</v>
       </c>
       <c r="P9">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+        <v>95</v>
+      </c>
+      <c r="Q9">
+        <v>90</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -1033,17 +1093,23 @@
         <v>71</v>
       </c>
       <c r="P10">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+      <c r="Q10">
+        <v>67</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11">
         <v>95</v>
@@ -1085,11 +1151,17 @@
         <v>88</v>
       </c>
       <c r="P11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="Q11">
+        <v>88</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1137,17 +1209,23 @@
         <v>103</v>
       </c>
       <c r="P12">
+        <v>103</v>
+      </c>
+      <c r="Q12">
+        <v>103</v>
+      </c>
+      <c r="R12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C13">
         <v>112</v>
@@ -1189,11 +1267,17 @@
         <v>109</v>
       </c>
       <c r="P13">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+      <c r="Q13">
+        <v>104</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1241,11 +1325,17 @@
         <v>54</v>
       </c>
       <c r="P14">
+        <v>54</v>
+      </c>
+      <c r="Q14">
+        <v>54</v>
+      </c>
+      <c r="R14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1293,11 +1383,17 @@
         <v>76</v>
       </c>
       <c r="P15">
+        <v>76</v>
+      </c>
+      <c r="Q15">
+        <v>76</v>
+      </c>
+      <c r="R15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1345,17 +1441,23 @@
         <v>93</v>
       </c>
       <c r="P16">
+        <v>93</v>
+      </c>
+      <c r="Q16">
+        <v>93</v>
+      </c>
+      <c r="R16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C17">
         <v>74</v>
@@ -1397,11 +1499,17 @@
         <v>75</v>
       </c>
       <c r="P17">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>67</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1449,11 +1557,17 @@
         <v>84</v>
       </c>
       <c r="P18">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+        <v>82</v>
+      </c>
+      <c r="Q18">
+        <v>82</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1501,11 +1615,17 @@
         <v>32</v>
       </c>
       <c r="P19">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+      <c r="Q19">
+        <v>29</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1553,17 +1673,23 @@
         <v>37</v>
       </c>
       <c r="P20">
+        <v>37</v>
+      </c>
+      <c r="Q20">
+        <v>37</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21">
         <v>32</v>
@@ -1605,11 +1731,17 @@
         <v>32</v>
       </c>
       <c r="P21">
+        <v>31</v>
+      </c>
+      <c r="Q21">
+        <v>31</v>
+      </c>
+      <c r="R21">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1657,11 +1789,17 @@
         <v>49</v>
       </c>
       <c r="P22">
+        <v>49</v>
+      </c>
+      <c r="Q22">
+        <v>49</v>
+      </c>
+      <c r="R22">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1709,11 +1847,17 @@
         <v>14</v>
       </c>
       <c r="P23">
+        <v>14</v>
+      </c>
+      <c r="Q23">
+        <v>14</v>
+      </c>
+      <c r="R23">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1761,11 +1905,17 @@
         <v>57</v>
       </c>
       <c r="P24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+      <c r="Q24">
+        <v>57</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1813,11 +1963,17 @@
         <v>67</v>
       </c>
       <c r="P25">
+        <v>67</v>
+      </c>
+      <c r="Q25">
+        <v>67</v>
+      </c>
+      <c r="R25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1865,11 +2021,17 @@
         <v>29</v>
       </c>
       <c r="P26">
+        <v>29</v>
+      </c>
+      <c r="Q26">
+        <v>29</v>
+      </c>
+      <c r="R26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1917,11 +2079,17 @@
         <v>29</v>
       </c>
       <c r="P27">
+        <v>29</v>
+      </c>
+      <c r="Q27">
+        <v>29</v>
+      </c>
+      <c r="R27">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1969,11 +2137,17 @@
         <v>66</v>
       </c>
       <c r="P28">
+        <v>66</v>
+      </c>
+      <c r="Q28">
+        <v>66</v>
+      </c>
+      <c r="R28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -2021,17 +2195,23 @@
         <v>47</v>
       </c>
       <c r="P29">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="Q29">
+        <v>48</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C30">
         <v>45</v>
@@ -2073,17 +2253,23 @@
         <v>45</v>
       </c>
       <c r="P30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+      <c r="Q30">
+        <v>45</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C31">
         <v>97</v>
@@ -2125,11 +2311,17 @@
         <v>87</v>
       </c>
       <c r="P31">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+      <c r="Q31">
+        <v>84</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -2177,11 +2369,17 @@
         <v>58</v>
       </c>
       <c r="P32">
+        <v>58</v>
+      </c>
+      <c r="Q32">
+        <v>58</v>
+      </c>
+      <c r="R32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -2229,11 +2427,17 @@
         <v>75</v>
       </c>
       <c r="P33">
+        <v>75</v>
+      </c>
+      <c r="Q33">
+        <v>75</v>
+      </c>
+      <c r="R33">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -2281,11 +2485,17 @@
         <v>59</v>
       </c>
       <c r="P34">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+      <c r="Q34">
+        <v>58</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -2333,17 +2543,23 @@
         <v>44</v>
       </c>
       <c r="P35">
+        <v>44</v>
+      </c>
+      <c r="Q35">
+        <v>44</v>
+      </c>
+      <c r="R35">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>33</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C36">
         <v>132</v>
@@ -2385,11 +2601,17 @@
         <v>130</v>
       </c>
       <c r="P36">
+        <v>129</v>
+      </c>
+      <c r="Q36">
+        <v>130</v>
+      </c>
+      <c r="R36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -2437,11 +2659,17 @@
         <v>146</v>
       </c>
       <c r="P37">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+      <c r="Q37">
+        <v>140</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -2489,11 +2717,17 @@
         <v>81</v>
       </c>
       <c r="P38">
+        <v>79</v>
+      </c>
+      <c r="Q38">
+        <v>81</v>
+      </c>
+      <c r="R38">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -2541,11 +2775,17 @@
         <v>96</v>
       </c>
       <c r="P39">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+      <c r="Q39">
+        <v>95</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -2593,17 +2833,23 @@
         <v>90</v>
       </c>
       <c r="P40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+      <c r="Q40">
+        <v>93</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>38</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C41">
         <v>91</v>
@@ -2645,11 +2891,17 @@
         <v>84</v>
       </c>
       <c r="P41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+      <c r="Q41">
+        <v>81</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -2697,11 +2949,17 @@
         <v>92</v>
       </c>
       <c r="P42">
+        <v>91</v>
+      </c>
+      <c r="Q42">
+        <v>92</v>
+      </c>
+      <c r="R42">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>40</v>
       </c>
@@ -2749,11 +3007,17 @@
         <v>124</v>
       </c>
       <c r="P43">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+      <c r="Q43">
+        <v>118</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>41</v>
       </c>
@@ -2801,11 +3065,17 @@
         <v>107</v>
       </c>
       <c r="P44">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+        <v>107</v>
+      </c>
+      <c r="Q44">
+        <v>107</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>42</v>
       </c>
@@ -2853,17 +3123,23 @@
         <v>122</v>
       </c>
       <c r="P45">
+        <v>122</v>
+      </c>
+      <c r="Q45">
+        <v>122</v>
+      </c>
+      <c r="R45">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>43</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C46">
         <v>137</v>
@@ -2905,17 +3181,23 @@
         <v>125</v>
       </c>
       <c r="P46">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+        <v>112</v>
+      </c>
+      <c r="Q46">
+        <v>112</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>44</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C47">
         <v>104</v>
@@ -2957,11 +3239,17 @@
         <v>98</v>
       </c>
       <c r="P47">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+      <c r="Q47">
+        <v>90</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>45</v>
       </c>
@@ -3009,11 +3297,17 @@
         <v>121</v>
       </c>
       <c r="P48">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+      <c r="Q48">
+        <v>115</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>46</v>
       </c>
@@ -3061,17 +3355,23 @@
         <v>120</v>
       </c>
       <c r="P49">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+        <v>115</v>
+      </c>
+      <c r="Q49">
+        <v>115</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>47</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C50">
         <v>135</v>
@@ -3113,17 +3413,23 @@
         <v>135</v>
       </c>
       <c r="P50">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+      <c r="Q50">
+        <v>124</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>48</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51">
         <v>109</v>
@@ -3165,11 +3471,17 @@
         <v>94</v>
       </c>
       <c r="P51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+      <c r="Q51">
+        <v>94</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>49</v>
       </c>
@@ -3217,11 +3529,17 @@
         <v>122</v>
       </c>
       <c r="P52">
+        <v>122</v>
+      </c>
+      <c r="Q52">
+        <v>123</v>
+      </c>
+      <c r="R52">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>50</v>
       </c>
@@ -3269,17 +3587,23 @@
         <v>119</v>
       </c>
       <c r="P53">
+        <v>119</v>
+      </c>
+      <c r="Q53">
+        <v>119</v>
+      </c>
+      <c r="R53">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>51</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C54">
         <v>195</v>
@@ -3321,17 +3645,23 @@
         <v>171</v>
       </c>
       <c r="P54">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.45">
+        <v>170</v>
+      </c>
+      <c r="Q54">
+        <v>168</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>52</v>
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C55">
         <v>157</v>
@@ -3373,11 +3703,17 @@
         <v>150</v>
       </c>
       <c r="P55">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.45">
+        <v>141</v>
+      </c>
+      <c r="Q55">
+        <v>141</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>53</v>
       </c>
@@ -3425,17 +3761,23 @@
         <v>102</v>
       </c>
       <c r="P56">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.45">
+        <v>101</v>
+      </c>
+      <c r="Q56">
+        <v>105</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>54</v>
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C57">
         <v>121</v>
@@ -3477,11 +3819,17 @@
         <v>113</v>
       </c>
       <c r="P57">
+        <v>111</v>
+      </c>
+      <c r="Q57">
+        <v>110</v>
+      </c>
+      <c r="R57">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>55</v>
       </c>
@@ -3529,17 +3877,23 @@
         <v>111</v>
       </c>
       <c r="P58">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.45">
+        <v>111</v>
+      </c>
+      <c r="Q58">
+        <v>111</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>56</v>
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C59">
         <v>141</v>
@@ -3581,11 +3935,17 @@
         <v>121</v>
       </c>
       <c r="P59">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+      <c r="Q59">
+        <v>124</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>57</v>
       </c>
@@ -3633,11 +3993,17 @@
         <v>131</v>
       </c>
       <c r="P60">
+        <v>131</v>
+      </c>
+      <c r="Q60">
+        <v>131</v>
+      </c>
+      <c r="R60">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.45">
       <c r="C61">
         <v>93.396551724137893</v>
       </c>
@@ -3646,7 +4012,7 @@
         <v>92.068965517241381</v>
       </c>
       <c r="E61">
-        <f t="shared" ref="E61:P61" si="2">AVERAGE(E3:E60)</f>
+        <f t="shared" ref="E61:R61" si="2">AVERAGE(E3:E60)</f>
         <v>92.793103448275858</v>
       </c>
       <c r="F61">
@@ -3687,17 +4053,23 @@
         <v>87.465517241379303</v>
       </c>
       <c r="P61">
+        <v>85.758620689655103</v>
+      </c>
+      <c r="Q61">
+        <v>85.379310344827502</v>
+      </c>
+      <c r="R61">
         <f t="shared" si="2"/>
-        <v>2.2413793103448274</v>
+        <v>1.103448275862069</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:O60 C62:O1048576 C61:P61">
+  <conditionalFormatting sqref="C1:Q60 C62:Q1048576 C61:R61">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>INDIRECT(ADDRESS(ROW(), 2)) = INDIRECT(ADDRESS(ROW(), COLUMN()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C4:O4">
+  <conditionalFormatting sqref="C4:Q4">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>$B$3</formula>
     </cfRule>

</xml_diff>